<commit_message>
Modified Git commnands File
</commit_message>
<xml_diff>
--- a/GitCommands.xlsx
+++ b/GitCommands.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27016"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27018"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="295" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C188D445-A92B-40BA-94C1-15BF329AEB2A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{870488AC-3373-470F-8867-7884C9665FFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -134,7 +134,7 @@
     <t>git status</t>
   </si>
   <si>
-    <t>Git Commit</t>
+    <t>Git Commit -commit changes</t>
   </si>
   <si>
     <t>git commit -m "message"</t>
@@ -279,7 +279,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -295,17 +295,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -626,8 +622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -637,103 +633,103 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="8"/>
-      <c r="R1" s="8"/>
-      <c r="S1" s="8"/>
-      <c r="T1" s="8"/>
-      <c r="U1" s="8"/>
-      <c r="V1" s="8"/>
-      <c r="W1" s="8"/>
-      <c r="X1" s="8"/>
-      <c r="Y1" s="8"/>
-      <c r="Z1" s="8"/>
-      <c r="AA1" s="8"/>
-      <c r="AB1" s="8"/>
-      <c r="AC1" s="8"/>
-      <c r="AD1" s="8"/>
-      <c r="AE1" s="8"/>
-      <c r="AF1" s="8"/>
-      <c r="AG1" s="8"/>
-      <c r="AH1" s="8"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="7"/>
+      <c r="V1" s="7"/>
+      <c r="W1" s="7"/>
+      <c r="X1" s="7"/>
+      <c r="Y1" s="7"/>
+      <c r="Z1" s="7"/>
+      <c r="AA1" s="7"/>
+      <c r="AB1" s="7"/>
+      <c r="AC1" s="7"/>
+      <c r="AD1" s="7"/>
+      <c r="AE1" s="7"/>
+      <c r="AF1" s="7"/>
+      <c r="AG1" s="7"/>
+      <c r="AH1" s="7"/>
       <c r="AI1" s="1"/>
     </row>
-    <row r="2" spans="1:35" s="7" customFormat="1">
-      <c r="A2" s="12">
+    <row r="2" spans="1:35" s="2" customFormat="1">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="10" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:35">
-      <c r="A3" s="12">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="9"/>
-      <c r="P3" s="9"/>
-      <c r="Q3" s="9"/>
-      <c r="R3" s="9"/>
-      <c r="S3" s="9"/>
-      <c r="T3" s="9"/>
-      <c r="U3" s="9"/>
-      <c r="V3" s="9"/>
-      <c r="W3" s="9"/>
-      <c r="X3" s="9"/>
-      <c r="Y3" s="9"/>
-      <c r="Z3" s="9"/>
-      <c r="AA3" s="9"/>
-      <c r="AB3" s="9"/>
-      <c r="AC3" s="9"/>
-      <c r="AD3" s="9"/>
-      <c r="AE3" s="9"/>
-      <c r="AF3" s="9"/>
-      <c r="AG3" s="9"/>
-      <c r="AH3" s="9"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="8"/>
+      <c r="W3" s="8"/>
+      <c r="X3" s="8"/>
+      <c r="Y3" s="8"/>
+      <c r="Z3" s="8"/>
+      <c r="AA3" s="8"/>
+      <c r="AB3" s="8"/>
+      <c r="AC3" s="8"/>
+      <c r="AD3" s="8"/>
+      <c r="AE3" s="8"/>
+      <c r="AF3" s="8"/>
+      <c r="AG3" s="8"/>
+      <c r="AH3" s="8"/>
     </row>
     <row r="4" spans="1:35" ht="30.75">
-      <c r="A4" s="12">
+      <c r="A4" s="4">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -775,7 +771,7 @@
       <c r="AH4" s="2"/>
     </row>
     <row r="5" spans="1:35">
-      <c r="A5" s="12">
+      <c r="A5" s="4">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -817,7 +813,7 @@
       <c r="AH5" s="2"/>
     </row>
     <row r="6" spans="1:35" ht="30.75">
-      <c r="A6" s="12">
+      <c r="A6" s="4">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -859,7 +855,7 @@
       <c r="AH6" s="2"/>
     </row>
     <row r="7" spans="1:35">
-      <c r="A7" s="13">
+      <c r="A7" s="11">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -901,7 +897,7 @@
       <c r="AH7" s="2"/>
     </row>
     <row r="8" spans="1:35">
-      <c r="A8" s="13">
+      <c r="A8" s="11">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -943,7 +939,7 @@
       <c r="AH8" s="2"/>
     </row>
     <row r="9" spans="1:35">
-      <c r="A9" s="13">
+      <c r="A9" s="11">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -985,7 +981,7 @@
       <c r="AH9" s="2"/>
     </row>
     <row r="10" spans="1:35">
-      <c r="A10" s="13">
+      <c r="A10" s="11">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -1027,7 +1023,7 @@
       <c r="AH10" s="2"/>
     </row>
     <row r="11" spans="1:35">
-      <c r="A11" s="13">
+      <c r="A11" s="11">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -1069,7 +1065,7 @@
       <c r="AH11" s="2"/>
     </row>
     <row r="12" spans="1:35">
-      <c r="A12" s="13">
+      <c r="A12" s="11">
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -1111,7 +1107,7 @@
       <c r="AH12" s="2"/>
     </row>
     <row r="13" spans="1:35">
-      <c r="A13" s="13">
+      <c r="A13" s="11">
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -1153,7 +1149,7 @@
       <c r="AH13" s="2"/>
     </row>
     <row r="14" spans="1:35">
-      <c r="A14" s="13">
+      <c r="A14" s="11">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -1195,7 +1191,7 @@
       <c r="AH14" s="2"/>
     </row>
     <row r="15" spans="1:35">
-      <c r="A15" s="13">
+      <c r="A15" s="11">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -1237,7 +1233,7 @@
       <c r="AH15" s="2"/>
     </row>
     <row r="16" spans="1:35">
-      <c r="A16" s="13">
+      <c r="A16" s="11">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -1279,7 +1275,7 @@
       <c r="AH16" s="2"/>
     </row>
     <row r="17" spans="1:34">
-      <c r="A17" s="13">
+      <c r="A17" s="11">
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -1321,7 +1317,7 @@
       <c r="AH17" s="2"/>
     </row>
     <row r="18" spans="1:34">
-      <c r="A18" s="13">
+      <c r="A18" s="11">
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -1363,7 +1359,7 @@
       <c r="AH18" s="2"/>
     </row>
     <row r="19" spans="1:34" ht="106.5">
-      <c r="A19" s="13">
+      <c r="A19" s="11">
         <v>18</v>
       </c>
       <c r="B19" s="5" t="s">
@@ -1405,7 +1401,7 @@
       <c r="AH19" s="2"/>
     </row>
     <row r="20" spans="1:34">
-      <c r="A20" s="13">
+      <c r="A20" s="11">
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -1447,7 +1443,7 @@
       <c r="AH20" s="2"/>
     </row>
     <row r="21" spans="1:34" ht="45.75">
-      <c r="A21" s="13">
+      <c r="A21" s="11">
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
@@ -1489,7 +1485,7 @@
       <c r="AH21" s="2"/>
     </row>
     <row r="22" spans="1:34" ht="30.75">
-      <c r="A22" s="13">
+      <c r="A22" s="11">
         <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
@@ -1531,7 +1527,7 @@
       <c r="AH22" s="2"/>
     </row>
     <row r="23" spans="1:34" ht="45.75">
-      <c r="A23" s="13">
+      <c r="A23" s="11">
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">

</xml_diff>